<commit_message>
Updates During The Period Till 05-04-2025
</commit_message>
<xml_diff>
--- a/Excel Examples Including  add-in xlwings and connected python - vba - dlls, etc/SCAN function example - Running sum resetting.xlsx
+++ b/Excel Examples Including  add-in xlwings and connected python - vba - dlls, etc/SCAN function example - Running sum resetting.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28720"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://carvart-my.sharepoint.com/personal/dhawal_carvart_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - 0yt2k\Excel Examples Including  add-in xlwings and connected python - vba - dlls, etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{25C336F7-83DD-4376-A65F-640E4C0DA407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E989168-26BB-426C-B8B9-D609F41AC0FF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B09942A-58B5-4B9D-BBAE-6B26EA05B044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D130C0E-DEB4-4978-A04E-62E7F9127D73}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{8D130C0E-DEB4-4978-A04E-62E7F9127D73}"/>
   </bookViews>
   <sheets>
     <sheet name="SCAN To accumulate With Reset" sheetId="1" r:id="rId1"/>
-    <sheet name="SCAN To workingout balance" sheetId="2" r:id="rId2"/>
+    <sheet name="SCAN accmu Real UseCase" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD596DAD-628E-4852-AB1B-4917CEB10AE1}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,9 +830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DD1794-A424-4520-B53D-907210580FC9}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Updated examples / scripts till 24-08-2025
</commit_message>
<xml_diff>
--- a/Excel Examples Including  add-in xlwings and connected python - vba - dlls, etc/SCAN function example - Running sum resetting.xlsx
+++ b/Excel Examples Including  add-in xlwings and connected python - vba - dlls, etc/SCAN function example - Running sum resetting.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28613"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - 0yt2k\Excel Examples Including  add-in xlwings and connected python - vba - dlls, etc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://carvart-my.sharepoint.com/personal/dhawal_carvart_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B09942A-58B5-4B9D-BBAE-6B26EA05B044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{25C336F7-83DD-4376-A65F-640E4C0DA407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E989168-26BB-426C-B8B9-D609F41AC0FF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{8D130C0E-DEB4-4978-A04E-62E7F9127D73}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D130C0E-DEB4-4978-A04E-62E7F9127D73}"/>
   </bookViews>
   <sheets>
     <sheet name="SCAN To accumulate With Reset" sheetId="1" r:id="rId1"/>
-    <sheet name="SCAN accmu Real UseCase" sheetId="2" r:id="rId2"/>
+    <sheet name="SCAN To workingout balance" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD596DAD-628E-4852-AB1B-4917CEB10AE1}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,7 +830,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DD1794-A424-4520-B53D-907210580FC9}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>